<commit_message>
Added FERT, and also updated the others with corrections
</commit_message>
<xml_diff>
--- a/CYTO_results.xlsx
+++ b/CYTO_results.xlsx
@@ -71,6 +71,12 @@
     <t>Microscopic observation [Identifier] in Body fluid by Cyto stain</t>
   </si>
   <si>
+    <t>18328-5</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Body fluid by Other stain</t>
+  </si>
+  <si>
     <t>47523-6</t>
   </si>
   <si>
@@ -80,12 +86,6 @@
     <t>Cytology report of Body fluid Cyto stain</t>
   </si>
   <si>
-    <t>18328-5</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Body fluid by Other stain</t>
-  </si>
-  <si>
     <t>MicroCyto|Body fld_BLANKROW</t>
   </si>
   <si>
@@ -131,12 +131,45 @@
     <t>Microscopic observation [Identifier] in Cervix by Cyto stain</t>
   </si>
   <si>
+    <t>18500-9</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Cervix by Cyto stain.thin prep</t>
+  </si>
+  <si>
+    <t>19765-7</t>
+  </si>
+  <si>
+    <t>Cvx/Vag</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Cervical or vaginal smear or scraping by Cyto stain</t>
+  </si>
+  <si>
+    <t>19766-5</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Cervical or vaginal smear or scraping by Cyto stain Narrative</t>
+  </si>
+  <si>
+    <t>32151-3</t>
+  </si>
+  <si>
+    <t>Vag</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Vaginal fluid by Non-gynecological cytology method</t>
+  </si>
+  <si>
+    <t>39086-4</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Vaginal fluid by Cyto stain.thin prep</t>
+  </si>
+  <si>
     <t>47527-7</t>
   </si>
   <si>
-    <t>Cvx/Vag</t>
-  </si>
-  <si>
     <t>Cytology report of Cervical or vaginal smear or scraping Cyto stain.thin prep</t>
   </si>
   <si>
@@ -146,39 +179,6 @@
     <t>Cytology report of Cervical or vaginal smear or scraping Cyto stain</t>
   </si>
   <si>
-    <t>32151-3</t>
-  </si>
-  <si>
-    <t>Vag</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Vaginal fluid by Non-gynecological cytology method</t>
-  </si>
-  <si>
-    <t>18500-9</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Cervix by Cyto stain.thin prep</t>
-  </si>
-  <si>
-    <t>39086-4</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Vaginal fluid by Cyto stain.thin prep</t>
-  </si>
-  <si>
-    <t>19765-7</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Cervical or vaginal smear or scraping by Cyto stain</t>
-  </si>
-  <si>
-    <t>19766-5</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Cervical or vaginal smear or scraping by Cyto stain Narrative</t>
-  </si>
-  <si>
     <t>MicroCyto|Genital-Female_BLANKROW</t>
   </si>
   <si>
@@ -209,27 +209,33 @@
     <t>6</t>
   </si>
   <si>
+    <t>10526-2</t>
+  </si>
+  <si>
+    <t>Sputum</t>
+  </si>
+  <si>
+    <t>Resp-Lower</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Sputum by Cyto stain</t>
+  </si>
+  <si>
+    <t>42210-5</t>
+  </si>
+  <si>
+    <t>Bronchial</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Bronchial specimen by Cyto stain</t>
+  </si>
+  <si>
     <t>47520-2</t>
   </si>
   <si>
-    <t>Sputum</t>
-  </si>
-  <si>
-    <t>Resp-Lower</t>
-  </si>
-  <si>
     <t>Cytology report of Sputum Cyto stain</t>
   </si>
   <si>
-    <t>42210-5</t>
-  </si>
-  <si>
-    <t>Bronchial</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Bronchial specimen by Cyto stain</t>
-  </si>
-  <si>
     <t>50007-4</t>
   </si>
   <si>
@@ -239,27 +245,21 @@
     <t>Cytology report of Bronchoalveolar lavage Cyto stain</t>
   </si>
   <si>
+    <t>50389-6</t>
+  </si>
+  <si>
+    <t>Bronchial brush</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Bronchial brush by Cyto stain.thin prep</t>
+  </si>
+  <si>
     <t>50971-1</t>
   </si>
   <si>
-    <t>Bronchial brush</t>
-  </si>
-  <si>
     <t>Cytology report of Bronchial brush Cyto stain</t>
   </si>
   <si>
-    <t>50389-6</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Bronchial brush by Cyto stain.thin prep</t>
-  </si>
-  <si>
-    <t>10526-2</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Sputum by Cyto stain</t>
-  </si>
-  <si>
     <t>MicroCyto|Resp-Lower_BLANKROW</t>
   </si>
   <si>
@@ -287,21 +287,21 @@
     <t>MicroCyto|Tiss</t>
   </si>
   <si>
+    <t>10527-0</t>
+  </si>
+  <si>
+    <t>Tiss</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Tissue by Cyto stain</t>
+  </si>
+  <si>
     <t>47529-3</t>
   </si>
   <si>
-    <t>Tiss</t>
-  </si>
-  <si>
     <t>Cytology report of Tissue Other stain</t>
   </si>
   <si>
-    <t>10527-0</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Tissue by Cyto stain</t>
-  </si>
-  <si>
     <t>MicroCyto|Tiss_BLANKROW</t>
   </si>
   <si>
@@ -329,46 +329,46 @@
     <t>MicroCyto|XXX</t>
   </si>
   <si>
+    <t>10525-4</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Unspecified specimen by Cyto stain</t>
+  </si>
+  <si>
+    <t>32785-8</t>
+  </si>
+  <si>
+    <t>Microscopic observation [Identifier] in Unspecified specimen by Non-gynecological cytology method</t>
+  </si>
+  <si>
     <t>47526-9</t>
   </si>
   <si>
-    <t>XXX</t>
-  </si>
-  <si>
     <t>Cytology report of Unspecified specimen Cyto stain</t>
   </si>
   <si>
-    <t>32785-8</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Unspecified specimen by Non-gynecological cytology method</t>
-  </si>
-  <si>
-    <t>10525-4</t>
-  </si>
-  <si>
-    <t>Microscopic observation [Identifier] in Unspecified specimen by Cyto stain</t>
-  </si>
-  <si>
     <t>MicroCyto|XXX_BLANKROW</t>
   </si>
   <si>
     <t>Specimen source|Genital-Female</t>
   </si>
   <si>
+    <t>19763-2</t>
+  </si>
+  <si>
+    <t>Specimen source</t>
+  </si>
+  <si>
+    <t>Specimen source [Identifier] in Cervical or vaginal smear or scraping by Cyto stain</t>
+  </si>
+  <si>
     <t>19770-7</t>
   </si>
   <si>
-    <t>Specimen source</t>
-  </si>
-  <si>
     <t>Deprecated Specimen source [Identifier] in Cervical or vaginal smear or scraping by Cyto stain</t>
-  </si>
-  <si>
-    <t>19763-2</t>
-  </si>
-  <si>
-    <t>Specimen source [Identifier] in Cervical or vaginal smear or scraping by Cyto stain</t>
   </si>
   <si>
     <t>Specimen source|Genital-Female_BLANKROW</t>
@@ -1459,7 +1459,8 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,7 +1477,7 @@
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1571,7 +1572,7 @@
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -1585,10 +1586,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -1668,7 +1669,7 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -1748,19 +1749,19 @@
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H13" t="s">
         <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
         <v>32</v>
@@ -1774,16 +1775,16 @@
         <v>32</v>
       </c>
       <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
         <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" t="s">
-        <v>39</v>
       </c>
       <c r="H14" t="s">
         <v>36</v>
@@ -1812,13 +1813,13 @@
         <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
       </c>
       <c r="I15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J15" t="s">
         <v>32</v>
@@ -1832,7 +1833,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -1841,7 +1842,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="H16" t="s">
         <v>36</v>
@@ -1870,7 +1871,7 @@
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H17" t="s">
         <v>36</v>
@@ -1893,13 +1894,13 @@
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
@@ -1922,13 +1923,13 @@
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -2002,7 +2003,7 @@
         <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
@@ -2053,7 +2054,7 @@
         <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -2111,19 +2112,19 @@
         <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H28" t="s">
         <v>66</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J28" t="s">
         <v>62</v>
@@ -2137,22 +2138,22 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" t="s">
         <v>74</v>
-      </c>
-      <c r="D29" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" t="s">
-        <v>75</v>
       </c>
       <c r="H29" t="s">
         <v>66</v>
       </c>
       <c r="I29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J29" t="s">
         <v>62</v>
@@ -2166,7 +2167,7 @@
         <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -2175,7 +2176,7 @@
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H30" t="s">
         <v>66</v>
@@ -2198,13 +2199,13 @@
         <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H31" t="s">
         <v>66</v>
@@ -2278,7 +2279,7 @@
         <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -2329,7 +2330,7 @@
         <v>90</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -2358,7 +2359,7 @@
         <v>93</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E39" t="s">
         <v>15</v>
@@ -2438,7 +2439,7 @@
         <v>100</v>
       </c>
       <c r="D43" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
@@ -2489,7 +2490,7 @@
         <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
@@ -2547,7 +2548,7 @@
         <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
@@ -2604,7 +2605,7 @@
         <v>114</v>
       </c>
       <c r="G51" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H51" t="s">
         <v>36</v>
@@ -2633,7 +2634,7 @@
         <v>114</v>
       </c>
       <c r="G52" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H52" t="s">
         <v>36</v>
@@ -2679,7 +2680,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2857,7 +2861,7 @@
         <v>133</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H9" t="s">
         <v>36</v>
@@ -2959,7 +2963,7 @@
         <v>142</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
         <v>36</v>
@@ -3010,7 +3014,7 @@
         <v>147</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
@@ -3288,7 +3292,7 @@
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
@@ -3300,7 +3304,7 @@
         <v>16</v>
       </c>
       <c r="I34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J34" t="s">
         <v>10</v>
@@ -3314,10 +3318,10 @@
         <v>10</v>
       </c>
       <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
         <v>21</v>
-      </c>
-      <c r="D35" t="s">
-        <v>14</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
@@ -3368,7 +3372,7 @@
         <v>172</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
@@ -3448,7 +3452,7 @@
         <v>29</v>
       </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
@@ -3885,19 +3889,19 @@
         <v>38</v>
       </c>
       <c r="D67" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H67" t="s">
         <v>36</v>
       </c>
       <c r="I67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J67" t="s">
         <v>32</v>
@@ -3911,16 +3915,16 @@
         <v>32</v>
       </c>
       <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>14</v>
+      </c>
+      <c r="E68" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" t="s">
         <v>41</v>
-      </c>
-      <c r="D68" t="s">
-        <v>19</v>
-      </c>
-      <c r="E68" t="s">
-        <v>15</v>
-      </c>
-      <c r="G68" t="s">
-        <v>39</v>
       </c>
       <c r="H68" t="s">
         <v>36</v>
@@ -3949,13 +3953,13 @@
         <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H69" t="s">
         <v>36</v>
       </c>
       <c r="I69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J69" t="s">
         <v>32</v>
@@ -3969,7 +3973,7 @@
         <v>32</v>
       </c>
       <c r="C70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D70" t="s">
         <v>14</v>
@@ -3978,7 +3982,7 @@
         <v>15</v>
       </c>
       <c r="G70" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="H70" t="s">
         <v>36</v>
@@ -4007,7 +4011,7 @@
         <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H71" t="s">
         <v>36</v>
@@ -4030,13 +4034,13 @@
         <v>50</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E72" t="s">
         <v>15</v>
       </c>
       <c r="G72" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H72" t="s">
         <v>36</v>
@@ -4059,13 +4063,13 @@
         <v>52</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H73" t="s">
         <v>36</v>
@@ -4394,7 +4398,7 @@
         <v>59</v>
       </c>
       <c r="D92" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E92" t="s">
         <v>15</v>
@@ -4802,7 +4806,7 @@
         <v>64</v>
       </c>
       <c r="D116" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E116" t="s">
         <v>15</v>
@@ -4860,19 +4864,19 @@
         <v>71</v>
       </c>
       <c r="D118" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E118" t="s">
         <v>15</v>
       </c>
       <c r="G118" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="H118" t="s">
         <v>66</v>
       </c>
       <c r="I118" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J118" t="s">
         <v>62</v>
@@ -4886,22 +4890,22 @@
         <v>62</v>
       </c>
       <c r="C119" t="s">
+        <v>73</v>
+      </c>
+      <c r="D119" t="s">
+        <v>21</v>
+      </c>
+      <c r="E119" t="s">
+        <v>15</v>
+      </c>
+      <c r="G119" t="s">
         <v>74</v>
-      </c>
-      <c r="D119" t="s">
-        <v>19</v>
-      </c>
-      <c r="E119" t="s">
-        <v>15</v>
-      </c>
-      <c r="G119" t="s">
-        <v>75</v>
       </c>
       <c r="H119" t="s">
         <v>66</v>
       </c>
       <c r="I119" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J119" t="s">
         <v>62</v>
@@ -4915,7 +4919,7 @@
         <v>62</v>
       </c>
       <c r="C120" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D120" t="s">
         <v>14</v>
@@ -4924,7 +4928,7 @@
         <v>15</v>
       </c>
       <c r="G120" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H120" t="s">
         <v>66</v>
@@ -4947,13 +4951,13 @@
         <v>79</v>
       </c>
       <c r="D121" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E121" t="s">
         <v>15</v>
       </c>
       <c r="G121" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H121" t="s">
         <v>66</v>
@@ -5282,7 +5286,7 @@
         <v>86</v>
       </c>
       <c r="D140" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E140" t="s">
         <v>15</v>
@@ -5333,7 +5337,7 @@
         <v>90</v>
       </c>
       <c r="D143" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E143" t="s">
         <v>15</v>
@@ -5362,7 +5366,7 @@
         <v>93</v>
       </c>
       <c r="D144" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E144" t="s">
         <v>15</v>
@@ -5402,7 +5406,7 @@
         <v>296</v>
       </c>
       <c r="D146" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E146" t="s">
         <v>15</v>
@@ -5493,7 +5497,7 @@
         <v>100</v>
       </c>
       <c r="D151" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E151" t="s">
         <v>15</v>
@@ -5544,7 +5548,7 @@
         <v>104</v>
       </c>
       <c r="D154" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E154" t="s">
         <v>15</v>
@@ -5602,7 +5606,7 @@
         <v>109</v>
       </c>
       <c r="D156" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E156" t="s">
         <v>15</v>
@@ -5659,7 +5663,7 @@
         <v>302</v>
       </c>
       <c r="G159" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H159" t="s">
         <v>36</v>
@@ -5914,7 +5918,7 @@
         <v>325</v>
       </c>
       <c r="G174" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H174" t="s">
         <v>36</v>
@@ -5965,7 +5969,7 @@
         <v>330</v>
       </c>
       <c r="G177" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H177" t="s">
         <v>36</v>
@@ -6016,7 +6020,7 @@
         <v>335</v>
       </c>
       <c r="G180" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H180" t="s">
         <v>36</v>
@@ -6067,7 +6071,7 @@
         <v>340</v>
       </c>
       <c r="G183" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H183" t="s">
         <v>36</v>
@@ -6118,7 +6122,7 @@
         <v>345</v>
       </c>
       <c r="G186" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H186" t="s">
         <v>36</v>
@@ -6169,7 +6173,7 @@
         <v>114</v>
       </c>
       <c r="G189" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H189" t="s">
         <v>36</v>
@@ -6198,7 +6202,7 @@
         <v>114</v>
       </c>
       <c r="G190" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H190" t="s">
         <v>36</v>
@@ -6249,7 +6253,7 @@
         <v>350</v>
       </c>
       <c r="G193" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H193" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Update for LOINC 2.67
</commit_message>
<xml_diff>
--- a/CYTO_results.xlsx
+++ b/CYTO_results.xlsx
@@ -1139,7 +1139,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -1169,16 +1169,10 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1477,7 +1471,7 @@
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2659,15 +2653,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576 H1:H1048576">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>$C1=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>E1&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2682,7 +2676,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" sqref="A1:J197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,7 +2726,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
       <c r="I2" t="s">
@@ -2743,7 +2737,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
@@ -2772,7 +2766,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I4" t="s">
@@ -2783,7 +2777,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
       <c r="I5" t="s">
@@ -2794,7 +2788,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
@@ -2823,7 +2817,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I7" t="s">
@@ -2834,7 +2828,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>131</v>
       </c>
       <c r="I8" t="s">
@@ -2845,7 +2839,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
@@ -2874,7 +2868,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I10" t="s">
@@ -2885,7 +2879,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>136</v>
       </c>
       <c r="I11" t="s">
@@ -2896,7 +2890,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
@@ -2925,7 +2919,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I13" t="s">
@@ -2936,7 +2930,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>140</v>
       </c>
       <c r="I14" t="s">
@@ -2947,7 +2941,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
@@ -2976,7 +2970,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I16" t="s">
@@ -2987,7 +2981,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>145</v>
       </c>
       <c r="I17" t="s">
@@ -2998,7 +2992,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
@@ -3027,7 +3021,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I19" t="s">
@@ -3038,7 +3032,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>150</v>
       </c>
       <c r="I20" t="s">
@@ -3049,7 +3043,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B21" t="s">
@@ -3078,7 +3072,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I22" t="s">
@@ -3089,7 +3083,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>156</v>
       </c>
       <c r="I23" t="s">
@@ -3100,7 +3094,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B24" t="s">
@@ -3129,7 +3123,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I25" t="s">
@@ -3140,7 +3134,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>161</v>
       </c>
       <c r="I26" t="s">
@@ -3151,7 +3145,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B27" t="s">
@@ -3180,7 +3174,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I28" t="s">
@@ -3191,7 +3185,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>166</v>
       </c>
       <c r="I29" t="s">
@@ -3202,7 +3196,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B30" t="s">
@@ -3231,7 +3225,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I31" t="s">
@@ -3242,7 +3236,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I32" t="s">
@@ -3253,7 +3247,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B33" t="s">
@@ -3282,7 +3276,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B34" t="s">
@@ -3311,7 +3305,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B35" t="s">
@@ -3340,7 +3334,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I36" t="s">
@@ -3351,7 +3345,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>171</v>
       </c>
       <c r="I37" t="s">
@@ -3362,7 +3356,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B38" t="s">
@@ -3391,7 +3385,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I39" t="s">
@@ -3402,7 +3396,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I40" t="s">
@@ -3413,7 +3407,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B41" t="s">
@@ -3442,7 +3436,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B42" t="s">
@@ -3471,7 +3465,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I43" t="s">
@@ -3482,7 +3476,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>176</v>
       </c>
       <c r="I44" t="s">
@@ -3493,7 +3487,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B45" t="s">
@@ -3522,7 +3516,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I46" t="s">
@@ -3533,7 +3527,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>181</v>
       </c>
       <c r="I47" t="s">
@@ -3544,7 +3538,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B48" t="s">
@@ -3573,7 +3567,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I49" t="s">
@@ -3584,7 +3578,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>185</v>
       </c>
       <c r="I50" t="s">
@@ -3595,7 +3589,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B51" t="s">
@@ -3624,7 +3618,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I52" t="s">
@@ -3635,7 +3629,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>190</v>
       </c>
       <c r="I53" t="s">
@@ -3646,7 +3640,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B54" t="s">
@@ -3675,7 +3669,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I55" t="s">
@@ -3686,7 +3680,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="1" t="s">
         <v>195</v>
       </c>
       <c r="I56" t="s">
@@ -3697,7 +3691,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B57" t="s">
@@ -3726,7 +3720,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I58" t="s">
@@ -3737,7 +3731,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>200</v>
       </c>
       <c r="I59" t="s">
@@ -3748,7 +3742,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B60" t="s">
@@ -3777,7 +3771,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I61" t="s">
@@ -3788,7 +3782,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="1" t="s">
         <v>205</v>
       </c>
       <c r="I62" t="s">
@@ -3799,7 +3793,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B63" t="s">
@@ -3828,7 +3822,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I64" t="s">
@@ -3839,7 +3833,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>32</v>
       </c>
       <c r="I65" t="s">
@@ -3850,7 +3844,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B66" t="s">
@@ -3879,7 +3873,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B67" t="s">
@@ -3908,7 +3902,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B68" t="s">
@@ -3937,7 +3931,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B69" t="s">
@@ -3966,7 +3960,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B70" t="s">
@@ -3995,7 +3989,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B71" t="s">
@@ -4024,7 +4018,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B72" t="s">
@@ -4053,7 +4047,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B73" t="s">
@@ -4082,7 +4076,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I74" t="s">
@@ -4093,7 +4087,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="1" t="s">
         <v>210</v>
       </c>
       <c r="I75" t="s">
@@ -4104,7 +4098,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B76" t="s">
@@ -4133,7 +4127,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I77" t="s">
@@ -4144,7 +4138,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="1" t="s">
         <v>215</v>
       </c>
       <c r="I78" t="s">
@@ -4155,7 +4149,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B79" t="s">
@@ -4184,7 +4178,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I80" t="s">
@@ -4195,7 +4189,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="1" t="s">
         <v>220</v>
       </c>
       <c r="I81" t="s">
@@ -4206,7 +4200,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B82" t="s">
@@ -4235,7 +4229,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I83" t="s">
@@ -4246,7 +4240,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="1" t="s">
         <v>225</v>
       </c>
       <c r="I84" t="s">
@@ -4257,7 +4251,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B85" t="s">
@@ -4286,7 +4280,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I86" t="s">
@@ -4297,7 +4291,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="1" t="s">
         <v>230</v>
       </c>
       <c r="I87" t="s">
@@ -4308,7 +4302,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B88" t="s">
@@ -4337,7 +4331,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I89" t="s">
@@ -4348,7 +4342,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I90" t="s">
@@ -4359,7 +4353,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B91" t="s">
@@ -4388,7 +4382,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B92" t="s">
@@ -4417,7 +4411,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I93" t="s">
@@ -4428,7 +4422,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="1" t="s">
         <v>235</v>
       </c>
       <c r="I94" t="s">
@@ -4439,7 +4433,7 @@
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B95" t="s">
@@ -4468,7 +4462,7 @@
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I96" t="s">
@@ -4479,7 +4473,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="1" t="s">
         <v>240</v>
       </c>
       <c r="I97" t="s">
@@ -4490,7 +4484,7 @@
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B98" t="s">
@@ -4519,7 +4513,7 @@
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I99" t="s">
@@ -4530,7 +4524,7 @@
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="1" t="s">
         <v>245</v>
       </c>
       <c r="I100" t="s">
@@ -4541,7 +4535,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B101" t="s">
@@ -4570,7 +4564,7 @@
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I102" t="s">
@@ -4581,7 +4575,7 @@
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="1" t="s">
         <v>250</v>
       </c>
       <c r="I103" t="s">
@@ -4592,7 +4586,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B104" t="s">
@@ -4621,7 +4615,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I105" t="s">
@@ -4632,7 +4626,7 @@
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" s="1" t="s">
         <v>255</v>
       </c>
       <c r="I106" t="s">
@@ -4643,7 +4637,7 @@
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B107" t="s">
@@ -4672,7 +4666,7 @@
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I108" t="s">
@@ -4683,7 +4677,7 @@
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="1" t="s">
         <v>260</v>
       </c>
       <c r="I109" t="s">
@@ -4694,7 +4688,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B110" t="s">
@@ -4723,7 +4717,7 @@
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I111" t="s">
@@ -4734,7 +4728,7 @@
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="1" t="s">
         <v>265</v>
       </c>
       <c r="I112" t="s">
@@ -4745,7 +4739,7 @@
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B113" t="s">
@@ -4774,7 +4768,7 @@
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I114" t="s">
@@ -4785,7 +4779,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="1" t="s">
         <v>62</v>
       </c>
       <c r="I115" t="s">
@@ -4796,7 +4790,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B116" t="s">
@@ -4825,7 +4819,7 @@
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B117" t="s">
@@ -4854,7 +4848,7 @@
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B118" t="s">
@@ -4883,7 +4877,7 @@
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B119" t="s">
@@ -4912,7 +4906,7 @@
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B120" t="s">
@@ -4941,7 +4935,7 @@
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B121" t="s">
@@ -4970,7 +4964,7 @@
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I122" t="s">
@@ -4981,7 +4975,7 @@
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>270</v>
       </c>
       <c r="I123" t="s">
@@ -4992,7 +4986,7 @@
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="A124" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B124" t="s">
@@ -5021,7 +5015,7 @@
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I125" t="s">
@@ -5032,7 +5026,7 @@
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" s="1" t="s">
         <v>275</v>
       </c>
       <c r="I126" t="s">
@@ -5043,7 +5037,7 @@
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B127" t="s">
@@ -5072,7 +5066,7 @@
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="A128" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I128" t="s">
@@ -5083,7 +5077,7 @@
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="1" t="s">
         <v>280</v>
       </c>
       <c r="I129" t="s">
@@ -5094,7 +5088,7 @@
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B130" t="s">
@@ -5123,7 +5117,7 @@
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I131" t="s">
@@ -5134,7 +5128,7 @@
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="1" t="s">
         <v>285</v>
       </c>
       <c r="I132" t="s">
@@ -5145,7 +5139,7 @@
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B133" t="s">
@@ -5174,7 +5168,7 @@
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I134" t="s">
@@ -5185,7 +5179,7 @@
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="1" t="s">
         <v>290</v>
       </c>
       <c r="I135" t="s">
@@ -5196,7 +5190,7 @@
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B136" t="s">
@@ -5225,7 +5219,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I137" t="s">
@@ -5236,7 +5230,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" s="1" t="s">
         <v>82</v>
       </c>
       <c r="I138" t="s">
@@ -5247,7 +5241,7 @@
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B139" t="s">
@@ -5276,7 +5270,7 @@
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B140" t="s">
@@ -5305,7 +5299,7 @@
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I141" t="s">
@@ -5316,7 +5310,7 @@
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" s="1" t="s">
         <v>89</v>
       </c>
       <c r="I142" t="s">
@@ -5327,7 +5321,7 @@
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="A143" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B143" t="s">
@@ -5356,7 +5350,7 @@
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="A144" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B144" t="s">
@@ -5385,7 +5379,7 @@
       </c>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="A145" s="1" t="s">
         <v>295</v>
       </c>
       <c r="I145" t="s">
@@ -5396,7 +5390,7 @@
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="A146" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B146" t="s">
@@ -5425,7 +5419,7 @@
       </c>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="A147" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I147" t="s">
@@ -5436,7 +5430,7 @@
       </c>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="A148" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I148" t="s">
@@ -5447,7 +5441,7 @@
       </c>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="A149" s="1" t="s">
         <v>96</v>
       </c>
       <c r="I149" t="s">
@@ -5458,7 +5452,7 @@
       </c>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="A150" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B150" t="s">
@@ -5487,7 +5481,7 @@
       </c>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="A151" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B151" t="s">
@@ -5516,7 +5510,7 @@
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="A152" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I152" t="s">
@@ -5527,7 +5521,7 @@
       </c>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="A153" s="1" t="s">
         <v>103</v>
       </c>
       <c r="I153" t="s">
@@ -5538,7 +5532,7 @@
       </c>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="A154" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B154" t="s">
@@ -5567,7 +5561,7 @@
       </c>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="A155" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B155" t="s">
@@ -5596,7 +5590,7 @@
       </c>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="A156" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B156" t="s">
@@ -5625,7 +5619,7 @@
       </c>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="A157" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I157" t="s">
@@ -5636,7 +5630,7 @@
       </c>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="A158" s="1" t="s">
         <v>300</v>
       </c>
       <c r="I158" t="s">
@@ -5647,7 +5641,7 @@
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="A159" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B159" t="s">
@@ -5676,7 +5670,7 @@
       </c>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="A160" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I160" t="s">
@@ -5687,7 +5681,7 @@
       </c>
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="A161" s="1" t="s">
         <v>305</v>
       </c>
       <c r="I161" t="s">
@@ -5698,7 +5692,7 @@
       </c>
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="A162" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B162" t="s">
@@ -5727,7 +5721,7 @@
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="A163" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I163" t="s">
@@ -5738,7 +5732,7 @@
       </c>
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="A164" s="1" t="s">
         <v>311</v>
       </c>
       <c r="I164" t="s">
@@ -5749,7 +5743,7 @@
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="A165" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B165" t="s">
@@ -5778,7 +5772,7 @@
       </c>
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="A166" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I166" t="s">
@@ -5789,7 +5783,7 @@
       </c>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="A167" s="1" t="s">
         <v>315</v>
       </c>
       <c r="I167" t="s">
@@ -5800,7 +5794,7 @@
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="A168" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B168" t="s">
@@ -5829,7 +5823,7 @@
       </c>
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="A169" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I169" t="s">
@@ -5840,7 +5834,7 @@
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="A170" s="1" t="s">
         <v>319</v>
       </c>
       <c r="I170" t="s">
@@ -5851,7 +5845,7 @@
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="A171" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B171" t="s">
@@ -5880,7 +5874,7 @@
       </c>
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="A172" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I172" t="s">
@@ -5891,7 +5885,7 @@
       </c>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="A173" s="1" t="s">
         <v>323</v>
       </c>
       <c r="I173" t="s">
@@ -5902,7 +5896,7 @@
       </c>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="A174" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B174" t="s">
@@ -5931,7 +5925,7 @@
       </c>
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="A175" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I175" t="s">
@@ -5942,7 +5936,7 @@
       </c>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="A176" s="1" t="s">
         <v>328</v>
       </c>
       <c r="I176" t="s">
@@ -5953,7 +5947,7 @@
       </c>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="A177" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B177" t="s">
@@ -5982,7 +5976,7 @@
       </c>
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+      <c r="A178" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I178" t="s">
@@ -5993,7 +5987,7 @@
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
+      <c r="A179" s="1" t="s">
         <v>333</v>
       </c>
       <c r="I179" t="s">
@@ -6004,7 +5998,7 @@
       </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+      <c r="A180" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B180" t="s">
@@ -6033,7 +6027,7 @@
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
+      <c r="A181" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I181" t="s">
@@ -6044,7 +6038,7 @@
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+      <c r="A182" s="1" t="s">
         <v>338</v>
       </c>
       <c r="I182" t="s">
@@ -6055,7 +6049,7 @@
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
+      <c r="A183" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B183" t="s">
@@ -6084,7 +6078,7 @@
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
+      <c r="A184" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I184" t="s">
@@ -6095,7 +6089,7 @@
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
+      <c r="A185" s="1" t="s">
         <v>343</v>
       </c>
       <c r="I185" t="s">
@@ -6106,7 +6100,7 @@
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
+      <c r="A186" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B186" t="s">
@@ -6135,7 +6129,7 @@
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+      <c r="A187" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I187" t="s">
@@ -6146,7 +6140,7 @@
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
+      <c r="A188" s="1" t="s">
         <v>112</v>
       </c>
       <c r="I188" t="s">
@@ -6157,7 +6151,7 @@
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
+      <c r="A189" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B189" t="s">
@@ -6186,7 +6180,7 @@
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="A190" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B190" t="s">
@@ -6215,7 +6209,7 @@
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="A191" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I191" t="s">
@@ -6226,7 +6220,7 @@
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
+      <c r="A192" s="1" t="s">
         <v>348</v>
       </c>
       <c r="I192" t="s">
@@ -6237,7 +6231,7 @@
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
+      <c r="A193" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B193" t="s">
@@ -6266,7 +6260,7 @@
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
+      <c r="A194" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I194" t="s">
@@ -6277,7 +6271,7 @@
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
+      <c r="A195" s="1" t="s">
         <v>353</v>
       </c>
       <c r="I195" t="s">
@@ -6288,7 +6282,7 @@
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A196" t="s">
+      <c r="A196" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B196" t="s">
@@ -6317,7 +6311,7 @@
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
+      <c r="A197" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I197" t="s">
@@ -6328,17 +6322,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$B1=""</formula>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="expression" priority="1" stopIfTrue="1">
+      <formula>B1=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>E1&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576 H1:H1048576">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>$C1=""</formula>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="expression" priority="3" stopIfTrue="1">
+      <formula>D1=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>E1&lt;&gt;D1</formula>
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>H1&lt;&gt;G1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update for LOINC 2.68
</commit_message>
<xml_diff>
--- a/CYTO_results.xlsx
+++ b/CYTO_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28530" windowHeight="16395"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28530" windowHeight="16395" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="group size &gt; 1" sheetId="1" r:id="rId1"/>
-    <sheet name="all groups" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" name="group size &gt; 1" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="all groups" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -1097,19 +1097,19 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1141,36 +1141,34 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
+        <patternFill patternType="none"/>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.7999816888943144"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.7999816888943144"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.7999816888943144"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1452,12 +1450,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" hidden="1" customWidth="1"/>
@@ -1468,38 +1466,38 @@
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2653,20 +2651,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>$B1=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576 H1:H1048576">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$C1=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>E1&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -2674,12 +2672,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:J197"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" hidden="1" customWidth="1"/>
@@ -2690,38 +2688,38 @@
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6323,22 +6321,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="expression" priority="1" stopIfTrue="1">
+    <cfRule type="expression" priority="1">
       <formula>B1=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>E1&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="expression" priority="3" stopIfTrue="1">
+    <cfRule type="expression" priority="5">
       <formula>D1=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>H1&lt;&gt;G1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>